<commit_message>
added tdl files from all months
gm calc works except for feb (mad ids with times)

functions dont pick licor right
</commit_message>
<xml_diff>
--- a/tdl_files/test.xlsx
+++ b/tdl_files/test.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="255" windowWidth="27795" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="255" yWindow="255" windowWidth="27795" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="tdl_oct_ch1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -524,14 +524,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -877,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,8 +943,8 @@
         <v>0.57245370370370374</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f>TEXT(E2, "m/dd/yyyy ")&amp;TEXT(H2, "hh:mm:ss")</f>
-        <v>10/25/2013 13:44:20</v>
+        <f>TEXT(E2, "dd/mm/yyyy ")&amp;TEXT(H2, "hh:mm:ss")</f>
+        <v>25/10/2013 13:44:20</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -973,9 +972,9 @@
       <c r="H3" s="1">
         <v>0.57268518518518519</v>
       </c>
-      <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I65" si="0">TEXT(E3, "m/dd/yyyy ")&amp;TEXT(H3, "hh:mm:ss")</f>
-        <v>10/25/2013 13:44:40</v>
+      <c r="I3" s="4" t="str">
+        <f t="shared" ref="I3:I65" si="0">TEXT(E3, "dd/mm/yyyy ")&amp;TEXT(H3, "hh:mm:ss")</f>
+        <v>25/10/2013 13:44:40</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1003,9 +1002,9 @@
       <c r="H4" s="1">
         <v>0.57291666666666663</v>
       </c>
-      <c r="I4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:45:00</v>
+      <c r="I4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:45:00</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1033,9 +1032,9 @@
       <c r="H5" s="1">
         <v>0.57314814814814818</v>
       </c>
-      <c r="I5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:45:20</v>
+      <c r="I5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:45:20</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1063,9 +1062,9 @@
       <c r="H6" s="1">
         <v>0.57337962962962963</v>
       </c>
-      <c r="I6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:45:40</v>
+      <c r="I6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:45:40</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1093,9 +1092,9 @@
       <c r="H7" s="1">
         <v>0.57361111111111118</v>
       </c>
-      <c r="I7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:46:00</v>
+      <c r="I7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:46:00</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1123,9 +1122,9 @@
       <c r="H8" s="1">
         <v>0.57384259259259263</v>
       </c>
-      <c r="I8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:46:20</v>
+      <c r="I8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:46:20</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1153,9 +1152,9 @@
       <c r="H9" s="1">
         <v>0.57407407407407407</v>
       </c>
-      <c r="I9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:46:40</v>
+      <c r="I9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:46:40</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1183,9 +1182,9 @@
       <c r="H10" s="1">
         <v>0.57430555555555551</v>
       </c>
-      <c r="I10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:47:00</v>
+      <c r="I10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:47:00</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1213,9 +1212,9 @@
       <c r="H11" s="1">
         <v>0.57453703703703707</v>
       </c>
-      <c r="I11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:47:20</v>
+      <c r="I11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:47:20</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1243,9 +1242,9 @@
       <c r="H12" s="1">
         <v>0.57476851851851851</v>
       </c>
-      <c r="I12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:47:40</v>
+      <c r="I12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:47:40</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1273,9 +1272,9 @@
       <c r="H13" s="1">
         <v>0.57500000000000007</v>
       </c>
-      <c r="I13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:48:00</v>
+      <c r="I13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:48:00</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1303,9 +1302,9 @@
       <c r="H14" s="1">
         <v>0.57523148148148151</v>
       </c>
-      <c r="I14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:48:20</v>
+      <c r="I14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:48:20</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1333,9 +1332,9 @@
       <c r="H15" s="1">
         <v>0.57546296296296295</v>
       </c>
-      <c r="I15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:48:40</v>
+      <c r="I15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:48:40</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1363,9 +1362,9 @@
       <c r="H16" s="1">
         <v>0.5756944444444444</v>
       </c>
-      <c r="I16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:49:00</v>
+      <c r="I16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:49:00</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1393,9 +1392,9 @@
       <c r="H17" s="1">
         <v>0.57592592592592595</v>
       </c>
-      <c r="I17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:49:20</v>
+      <c r="I17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:49:20</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1423,9 +1422,9 @@
       <c r="H18" s="1">
         <v>0.5761574074074074</v>
       </c>
-      <c r="I18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:49:40</v>
+      <c r="I18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:49:40</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1453,9 +1452,9 @@
       <c r="H19" s="1">
         <v>0.57638888888888895</v>
       </c>
-      <c r="I19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:50:00</v>
+      <c r="I19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:50:00</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1483,9 +1482,9 @@
       <c r="H20" s="1">
         <v>0.57662037037037039</v>
       </c>
-      <c r="I20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:50:20</v>
+      <c r="I20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:50:20</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1513,9 +1512,9 @@
       <c r="H21" s="1">
         <v>0.57685185185185184</v>
       </c>
-      <c r="I21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:50:40</v>
+      <c r="I21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:50:40</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1543,9 +1542,9 @@
       <c r="H22" s="1">
         <v>0.57708333333333328</v>
       </c>
-      <c r="I22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:51:00</v>
+      <c r="I22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:51:00</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1573,9 +1572,9 @@
       <c r="H23" s="1">
         <v>0.57731481481481484</v>
       </c>
-      <c r="I23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:51:20</v>
+      <c r="I23" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:51:20</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1603,9 +1602,9 @@
       <c r="H24" s="1">
         <v>0.57754629629629628</v>
       </c>
-      <c r="I24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:51:40</v>
+      <c r="I24" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:51:40</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1633,9 +1632,9 @@
       <c r="H25" s="1">
         <v>0.57777777777777783</v>
       </c>
-      <c r="I25" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 13:52:00</v>
+      <c r="I25" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 13:52:00</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1663,9 +1662,9 @@
       <c r="H26" s="1">
         <v>0.59375</v>
       </c>
-      <c r="I26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:15:00</v>
+      <c r="I26" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:15:00</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1693,9 +1692,9 @@
       <c r="H27" s="1">
         <v>0.59398148148148155</v>
       </c>
-      <c r="I27" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:15:20</v>
+      <c r="I27" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:15:20</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1723,9 +1722,9 @@
       <c r="H28" s="1">
         <v>0.594212962962963</v>
       </c>
-      <c r="I28" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:15:40</v>
+      <c r="I28" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:15:40</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1753,9 +1752,9 @@
       <c r="H29" s="1">
         <v>0.59444444444444444</v>
       </c>
-      <c r="I29" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:16:00</v>
+      <c r="I29" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:16:00</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1783,9 +1782,9 @@
       <c r="H30" s="1">
         <v>0.59467592592592589</v>
       </c>
-      <c r="I30" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:16:20</v>
+      <c r="I30" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:16:20</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1813,9 +1812,9 @@
       <c r="H31" s="1">
         <v>0.59490740740740744</v>
       </c>
-      <c r="I31" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:16:40</v>
+      <c r="I31" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:16:40</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1843,9 +1842,9 @@
       <c r="H32" s="1">
         <v>0.59513888888888888</v>
       </c>
-      <c r="I32" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:17:00</v>
+      <c r="I32" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:17:00</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1873,9 +1872,9 @@
       <c r="H33" s="1">
         <v>0.59537037037037044</v>
       </c>
-      <c r="I33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:17:20</v>
+      <c r="I33" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:17:20</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1903,9 +1902,9 @@
       <c r="H34" s="1">
         <v>0.59560185185185188</v>
       </c>
-      <c r="I34" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:17:40</v>
+      <c r="I34" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:17:40</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1933,9 +1932,9 @@
       <c r="H35" s="1">
         <v>0.59583333333333333</v>
       </c>
-      <c r="I35" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:18:00</v>
+      <c r="I35" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:18:00</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1963,9 +1962,9 @@
       <c r="H36" s="1">
         <v>0.59606481481481477</v>
       </c>
-      <c r="I36" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:18:20</v>
+      <c r="I36" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:18:20</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1993,9 +1992,9 @@
       <c r="H37" s="1">
         <v>0.59629629629629632</v>
       </c>
-      <c r="I37" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:18:40</v>
+      <c r="I37" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:18:40</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2023,9 +2022,9 @@
       <c r="H38" s="1">
         <v>0.59652777777777777</v>
       </c>
-      <c r="I38" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:19:00</v>
+      <c r="I38" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:19:00</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2053,9 +2052,9 @@
       <c r="H39" s="1">
         <v>0.59675925925925932</v>
       </c>
-      <c r="I39" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:19:20</v>
+      <c r="I39" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:19:20</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2083,9 +2082,9 @@
       <c r="H40" s="1">
         <v>0.59699074074074077</v>
       </c>
-      <c r="I40" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:19:40</v>
+      <c r="I40" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:19:40</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2113,9 +2112,9 @@
       <c r="H41" s="1">
         <v>0.59722222222222221</v>
       </c>
-      <c r="I41" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:20:00</v>
+      <c r="I41" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:20:00</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2143,9 +2142,9 @@
       <c r="H42" s="1">
         <v>0.59745370370370365</v>
       </c>
-      <c r="I42" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:20:20</v>
+      <c r="I42" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:20:20</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2173,9 +2172,9 @@
       <c r="H43" s="1">
         <v>0.59768518518518521</v>
       </c>
-      <c r="I43" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:20:40</v>
+      <c r="I43" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:20:40</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2203,9 +2202,9 @@
       <c r="H44" s="1">
         <v>0.59791666666666665</v>
       </c>
-      <c r="I44" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:21:00</v>
+      <c r="I44" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:21:00</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2233,9 +2232,9 @@
       <c r="H45" s="1">
         <v>0.59814814814814821</v>
       </c>
-      <c r="I45" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:21:20</v>
+      <c r="I45" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:21:20</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2263,9 +2262,9 @@
       <c r="H46" s="1">
         <v>0.60763888888888895</v>
       </c>
-      <c r="I46" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:35:00</v>
+      <c r="I46" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:35:00</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2293,9 +2292,9 @@
       <c r="H47" s="1">
         <v>0.60787037037037039</v>
       </c>
-      <c r="I47" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:35:20</v>
+      <c r="I47" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:35:20</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2323,9 +2322,9 @@
       <c r="H48" s="1">
         <v>0.60810185185185184</v>
       </c>
-      <c r="I48" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:35:40</v>
+      <c r="I48" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:35:40</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2353,9 +2352,9 @@
       <c r="H49" s="1">
         <v>0.60833333333333328</v>
       </c>
-      <c r="I49" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:36:00</v>
+      <c r="I49" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:36:00</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2383,9 +2382,9 @@
       <c r="H50" s="1">
         <v>0.60856481481481484</v>
       </c>
-      <c r="I50" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:36:20</v>
+      <c r="I50" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:36:20</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2413,9 +2412,9 @@
       <c r="H51" s="1">
         <v>0.60879629629629628</v>
       </c>
-      <c r="I51" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:36:40</v>
+      <c r="I51" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:36:40</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2443,9 +2442,9 @@
       <c r="H52" s="1">
         <v>0.60902777777777783</v>
       </c>
-      <c r="I52" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:37:00</v>
+      <c r="I52" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:37:00</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2473,9 +2472,9 @@
       <c r="H53" s="1">
         <v>0.60925925925925928</v>
       </c>
-      <c r="I53" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:37:20</v>
+      <c r="I53" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:37:20</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2503,9 +2502,9 @@
       <c r="H54" s="1">
         <v>0.60949074074074072</v>
       </c>
-      <c r="I54" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:37:40</v>
+      <c r="I54" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:37:40</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2533,9 +2532,9 @@
       <c r="H55" s="1">
         <v>0.60972222222222217</v>
       </c>
-      <c r="I55" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:38:00</v>
+      <c r="I55" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:38:00</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2563,9 +2562,9 @@
       <c r="H56" s="1">
         <v>0.60995370370370372</v>
       </c>
-      <c r="I56" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:38:20</v>
+      <c r="I56" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:38:20</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2593,9 +2592,9 @@
       <c r="H57" s="1">
         <v>0.61018518518518516</v>
       </c>
-      <c r="I57" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:38:40</v>
+      <c r="I57" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:38:40</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2623,9 +2622,9 @@
       <c r="H58" s="1">
         <v>0.61041666666666672</v>
       </c>
-      <c r="I58" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:39:00</v>
+      <c r="I58" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:39:00</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2653,9 +2652,9 @@
       <c r="H59" s="1">
         <v>0.61064814814814816</v>
       </c>
-      <c r="I59" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:39:20</v>
+      <c r="I59" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:39:20</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2683,9 +2682,9 @@
       <c r="H60" s="1">
         <v>0.61087962962962961</v>
       </c>
-      <c r="I60" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:39:40</v>
+      <c r="I60" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:39:40</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2713,9 +2712,9 @@
       <c r="H61" s="1">
         <v>0.61111111111111105</v>
       </c>
-      <c r="I61" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:40:00</v>
+      <c r="I61" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:40:00</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2743,9 +2742,9 @@
       <c r="H62" s="1">
         <v>0.6113425925925926</v>
       </c>
-      <c r="I62" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:40:20</v>
+      <c r="I62" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:40:20</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2773,9 +2772,9 @@
       <c r="H63" s="1">
         <v>0.61157407407407405</v>
       </c>
-      <c r="I63" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:40:40</v>
+      <c r="I63" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:40:40</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2803,9 +2802,9 @@
       <c r="H64" s="1">
         <v>0.6118055555555556</v>
       </c>
-      <c r="I64" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:41:00</v>
+      <c r="I64" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:41:00</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2833,9 +2832,9 @@
       <c r="H65" s="1">
         <v>0.61203703703703705</v>
       </c>
-      <c r="I65" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>10/25/2013 14:41:20</v>
+      <c r="I65" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25/10/2013 14:41:20</v>
       </c>
     </row>
   </sheetData>
@@ -2845,865 +2844,479 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A2:AA76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="5"/>
+    <col min="4" max="13" width="9.140625" style="5" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="5"/>
+    <col min="16" max="16" width="14.85546875" style="5" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" style="5" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" style="5" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="0" style="5" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" style="6" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="5"/>
+    <col min="22" max="22" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="9.140625" style="5"/>
+    <col min="27" max="27" width="15.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="6"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="6"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="R2" s="4"/>
+      <c r="AA2" s="4"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="6"/>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="R3" s="4"/>
+      <c r="AA3" s="4"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="R4" s="4"/>
+      <c r="AA4" s="4"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="6"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="R5" s="4"/>
+      <c r="AA5" s="4"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="6"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="R6" s="4"/>
+      <c r="AA6" s="4"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="6"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="R7" s="4"/>
+      <c r="AA7" s="4"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="6"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="R8" s="4"/>
+      <c r="AA8" s="4"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="6"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="R9" s="4"/>
+      <c r="AA9" s="4"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="6"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="R10" s="4"/>
+      <c r="AA10" s="4"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="6"/>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="R11" s="4"/>
+      <c r="AA11" s="4"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="6"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="R12" s="4"/>
+      <c r="AA12" s="4"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="6"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="R13" s="4"/>
+      <c r="AA13" s="4"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="6"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="R14" s="4"/>
+      <c r="AA14" s="4"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="6"/>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="R15" s="4"/>
+      <c r="AA15" s="4"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="6"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="R16" s="4"/>
+      <c r="AA16" s="4"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="6"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="R17" s="4"/>
+      <c r="AA17" s="4"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="6"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="R18" s="4"/>
+      <c r="AA18" s="4"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="6"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="R19" s="4"/>
+      <c r="AA19" s="4"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="6"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="R20" s="4"/>
+      <c r="AA20" s="4"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="6"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="R21" s="4"/>
+      <c r="AA21" s="4"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="6"/>
-      <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="R22" s="4"/>
+      <c r="AA22" s="4"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="6"/>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="R23" s="4"/>
+      <c r="AA23" s="4"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="6"/>
-      <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="R24" s="4"/>
+      <c r="AA24" s="4"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="6"/>
-      <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="R25" s="4"/>
+      <c r="AA25" s="4"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="6"/>
-      <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="R26" s="4"/>
+      <c r="AA26" s="4"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="6"/>
-      <c r="J27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="R27" s="4"/>
+      <c r="AA27" s="4"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="6"/>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="R28" s="4"/>
+      <c r="AA28" s="4"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="6"/>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+      <c r="R29" s="4"/>
+      <c r="AA29" s="4"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="6"/>
-      <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+      <c r="R30" s="4"/>
+      <c r="AA30" s="4"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="6"/>
-      <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+      <c r="R31" s="4"/>
+      <c r="AA31" s="4"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
       <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="6"/>
-      <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="R32" s="4"/>
+      <c r="AA32" s="4"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="6"/>
-      <c r="J33" s="4"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="R33" s="4"/>
+      <c r="AA33" s="4"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="6"/>
-      <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
+      <c r="R34" s="4"/>
+      <c r="AA34" s="4"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="6"/>
-      <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+      <c r="R35" s="4"/>
+      <c r="AA35" s="4"/>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
       <c r="B36" s="4"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="6"/>
-      <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
+      <c r="R36" s="4"/>
+      <c r="AA36" s="4"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="6"/>
-      <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
+      <c r="R37" s="4"/>
+      <c r="AA37" s="4"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
       <c r="B38" s="4"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="6"/>
-      <c r="J38" s="4"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
+      <c r="R38" s="4"/>
+      <c r="AA38" s="4"/>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
       <c r="B39" s="4"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="6"/>
-      <c r="J39" s="4"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
+      <c r="R39" s="4"/>
+      <c r="AA39" s="4"/>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
       <c r="B40" s="4"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="6"/>
-      <c r="J40" s="4"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
+      <c r="R40" s="4"/>
+      <c r="AA40" s="4"/>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
       <c r="B41" s="4"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="6"/>
-      <c r="J41" s="4"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
+      <c r="R41" s="4"/>
+      <c r="AA41" s="4"/>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
       <c r="B42" s="4"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="6"/>
-      <c r="J42" s="4"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
+      <c r="R42" s="4"/>
+      <c r="AA42" s="4"/>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
       <c r="B43" s="4"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="6"/>
-      <c r="J43" s="4"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
+      <c r="R43" s="4"/>
+      <c r="AA43" s="4"/>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
       <c r="B44" s="4"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="6"/>
-      <c r="J44" s="4"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
+      <c r="R44" s="4"/>
+      <c r="AA44" s="4"/>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
       <c r="B45" s="4"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="6"/>
-      <c r="J45" s="4"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
+      <c r="R45" s="4"/>
+      <c r="AA45" s="4"/>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
       <c r="B46" s="4"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="6"/>
-      <c r="J46" s="4"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
+      <c r="R46" s="4"/>
+      <c r="AA46" s="4"/>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
       <c r="B47" s="4"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="6"/>
-      <c r="J47" s="4"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
+      <c r="R47" s="4"/>
+      <c r="AA47" s="4"/>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
       <c r="B48" s="4"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="6"/>
-      <c r="J48" s="4"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
+      <c r="R48" s="4"/>
+      <c r="AA48" s="4"/>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
       <c r="B49" s="4"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="6"/>
-      <c r="J49" s="4"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
+      <c r="R49" s="4"/>
+      <c r="AA49" s="4"/>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
       <c r="B50" s="4"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="6"/>
-      <c r="J50" s="4"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
+      <c r="R50" s="4"/>
+      <c r="AA50" s="4"/>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
       <c r="B51" s="4"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="6"/>
-      <c r="J51" s="4"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
+      <c r="R51" s="4"/>
+      <c r="AA51" s="4"/>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
       <c r="B52" s="4"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="6"/>
-      <c r="J52" s="4"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
+      <c r="R52" s="4"/>
+      <c r="AA52" s="4"/>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
       <c r="B53" s="4"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="6"/>
-      <c r="J53" s="4"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
+      <c r="R53" s="4"/>
+      <c r="AA53" s="4"/>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
       <c r="B54" s="4"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="6"/>
-      <c r="J54" s="4"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
+      <c r="R54" s="4"/>
+      <c r="AA54" s="4"/>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A55" s="6"/>
       <c r="B55" s="4"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="6"/>
-      <c r="J55" s="4"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
+      <c r="R55" s="4"/>
+      <c r="AA55" s="4"/>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
       <c r="B56" s="4"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="6"/>
-      <c r="J56" s="4"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
+      <c r="R56" s="4"/>
+      <c r="AA56" s="4"/>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
       <c r="B57" s="4"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="6"/>
-      <c r="J57" s="4"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
+      <c r="R57" s="4"/>
+      <c r="AA57" s="4"/>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A58" s="6"/>
       <c r="B58" s="4"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="6"/>
-      <c r="J58" s="4"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
+      <c r="R58" s="4"/>
+      <c r="AA58" s="4"/>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A59" s="6"/>
       <c r="B59" s="4"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="6"/>
-      <c r="J59" s="4"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
+      <c r="R59" s="4"/>
+      <c r="AA59" s="4"/>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A60" s="6"/>
       <c r="B60" s="4"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="6"/>
-      <c r="J60" s="4"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
+      <c r="R60" s="4"/>
+      <c r="AA60" s="4"/>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
       <c r="B61" s="4"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="6"/>
-      <c r="J61" s="4"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
+      <c r="R61" s="4"/>
+      <c r="AA61" s="4"/>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A62" s="6"/>
       <c r="B62" s="4"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="6"/>
-      <c r="J62" s="4"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
+      <c r="R62" s="4"/>
+      <c r="AA62" s="4"/>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A63" s="6"/>
       <c r="B63" s="4"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="6"/>
-      <c r="J63" s="4"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
+      <c r="R63" s="4"/>
+      <c r="AA63" s="4"/>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A64" s="6"/>
       <c r="B64" s="4"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="7"/>
-      <c r="H64" s="6"/>
-      <c r="J64" s="4"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
+      <c r="R64" s="4"/>
+      <c r="AA64" s="4"/>
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A65" s="6"/>
       <c r="B65" s="4"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="7"/>
-      <c r="H65" s="6"/>
-      <c r="J65" s="4"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
+      <c r="R65" s="4"/>
+      <c r="AA65" s="4"/>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A66" s="6"/>
       <c r="B66" s="4"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="6"/>
-      <c r="J66" s="4"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
+      <c r="R66" s="4"/>
+      <c r="AA66" s="4"/>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A67" s="6"/>
       <c r="B67" s="4"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="6"/>
-      <c r="J67" s="4"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
+      <c r="R67" s="4"/>
+      <c r="AA67" s="4"/>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A68" s="6"/>
       <c r="B68" s="4"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="7"/>
-      <c r="H68" s="6"/>
-      <c r="J68" s="4"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
+      <c r="R68" s="4"/>
+      <c r="AA68" s="4"/>
+    </row>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A69" s="6"/>
       <c r="B69" s="4"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="7"/>
-      <c r="H69" s="6"/>
-      <c r="J69" s="4"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="7"/>
+      <c r="R69" s="4"/>
+      <c r="AA69" s="4"/>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A70" s="6"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="6"/>
-      <c r="J70" s="4"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
+      <c r="R70" s="4"/>
+      <c r="AA70" s="4"/>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A71" s="6"/>
       <c r="B71" s="4"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="6"/>
-      <c r="J71" s="4"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
+      <c r="R71" s="4"/>
+      <c r="AA71" s="4"/>
+    </row>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
       <c r="B72" s="4"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="6"/>
-      <c r="J72" s="4"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
+      <c r="R72" s="4"/>
+      <c r="AA72" s="4"/>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A73" s="6"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="7"/>
-      <c r="H73" s="6"/>
-      <c r="J73" s="4"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="7"/>
+      <c r="R73" s="4"/>
+      <c r="AA73" s="4"/>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A74" s="6"/>
       <c r="B74" s="4"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="7"/>
-      <c r="H74" s="6"/>
-      <c r="J74" s="4"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
+      <c r="R74" s="4"/>
+      <c r="AA74" s="4"/>
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A75" s="6"/>
       <c r="B75" s="4"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="6"/>
-      <c r="J75" s="4"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="7"/>
+      <c r="R75" s="4"/>
+      <c r="AA75" s="4"/>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A76" s="6"/>
       <c r="B76" s="4"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="7"/>
-      <c r="H76" s="6"/>
-      <c r="J76" s="4"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="7"/>
-      <c r="H77" s="6"/>
-      <c r="J77" s="4"/>
+      <c r="R76" s="4"/>
+      <c r="AA76" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3727,310 +3340,310 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
+      <c r="A1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="6"/>
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="6"/>
       <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="6"/>
       <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="6"/>
       <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="A26" s="6"/>
       <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="6"/>
       <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="6"/>
       <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="A29" s="6"/>
       <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+      <c r="A30" s="6"/>
       <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+      <c r="A31" s="6"/>
       <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+      <c r="A32" s="6"/>
       <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="6"/>
       <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="A34" s="6"/>
       <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
+      <c r="A35" s="6"/>
       <c r="B35" s="4"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+      <c r="A36" s="6"/>
       <c r="B36" s="4"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
+      <c r="A37" s="6"/>
       <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
+      <c r="A38" s="6"/>
       <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
+      <c r="A39" s="6"/>
       <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
+      <c r="A40" s="6"/>
       <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
+      <c r="A41" s="6"/>
       <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
+      <c r="A42" s="6"/>
       <c r="B42" s="4"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
+      <c r="A43" s="6"/>
       <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
+      <c r="A44" s="6"/>
       <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
+      <c r="A45" s="6"/>
       <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
+      <c r="A46" s="6"/>
       <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
+      <c r="A47" s="6"/>
       <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
+      <c r="A48" s="6"/>
       <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
+      <c r="A49" s="6"/>
       <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
+      <c r="A50" s="6"/>
       <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
+      <c r="A51" s="6"/>
       <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
+      <c r="A52" s="6"/>
       <c r="B52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
+      <c r="A53" s="6"/>
       <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
+      <c r="A54" s="6"/>
       <c r="B54" s="4"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
+      <c r="A55" s="6"/>
       <c r="B55" s="4"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
+      <c r="A56" s="6"/>
       <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
+      <c r="A57" s="6"/>
       <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
+      <c r="A58" s="6"/>
       <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
+      <c r="A59" s="6"/>
       <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
+      <c r="A60" s="6"/>
       <c r="B60" s="4"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
+      <c r="A61" s="6"/>
       <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
+      <c r="A62" s="6"/>
       <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
+      <c r="A63" s="6"/>
       <c r="B63" s="4"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
+      <c r="A64" s="6"/>
       <c r="B64" s="4"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
+      <c r="A65" s="6"/>
       <c r="B65" s="4"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
+      <c r="A66" s="6"/>
       <c r="B66" s="4"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
+      <c r="A67" s="6"/>
       <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
+      <c r="A68" s="6"/>
       <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
+      <c r="A69" s="6"/>
       <c r="B69" s="4"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="7"/>
+      <c r="A70" s="6"/>
       <c r="B70" s="4"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
+      <c r="A71" s="6"/>
       <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
+      <c r="A72" s="6"/>
       <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
+      <c r="A73" s="6"/>
       <c r="B73" s="4"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="7"/>
+      <c r="A74" s="6"/>
       <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
+      <c r="A75" s="6"/>
       <c r="B75" s="4"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="7"/>
+      <c r="A76" s="6"/>
       <c r="B76" s="4"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
+      <c r="A77" s="6"/>
       <c r="B77" s="4"/>
     </row>
   </sheetData>

</xml_diff>